<commit_message>
Update foraging patch hardware doc
</commit_message>
<xml_diff>
--- a/src/downloads/Foraging-Patch-BOM.xlsx
+++ b/src/downloads/Foraging-Patch-BOM.xlsx
@@ -5,15 +5,15 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/412ba1c02c359b1c/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcalc\UCL Dropbox\Lorenza Calcaterra\Project_aeon\Assembly instructions\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{5049CA79-1E51-4C0B-9C8F-9497E3DA38C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F90A9FA6-6850-4C60-80D6-961F114AC47E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF494D9-4B22-4719-887A-C80003F011C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38A5E6C9-8D94-40D2-9BFA-B29F5FB44878}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feeder" sheetId="3" r:id="rId1"/>
+    <sheet name="AEON Feeder" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,44 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Lorenza Calcaterra</author>
-  </authors>
-  <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{EF889EDA-5804-4EB4-9EBB-1F5D632C2E24}">
-      <text/>
-    </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{87F21182-8E0A-403E-B42C-2342DC3F76EA}">
-      <text/>
-    </comment>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{14503D7F-3F9C-4269-9DA8-1D1A15D4BA7C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{6F2DC094-F40F-4E2C-B647-E2E15F32BE0E}">
-      <text/>
-    </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{5CCB3F11-C5AF-4186-97A6-A0003DD56BA7}">
-      <text/>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="108">
   <si>
     <t xml:space="preserve">Inventory list </t>
   </si>
@@ -119,9 +83,6 @@
     <t>Neodymium magnet</t>
   </si>
   <si>
-    <t>tube conains 10 magnets - 2 per feeder needed</t>
-  </si>
-  <si>
     <t>Shoulder bolt</t>
   </si>
   <si>
@@ -167,9 +128,6 @@
     <t>bag of 50 - feeder to hex tile</t>
   </si>
   <si>
-    <t>521-957</t>
-  </si>
-  <si>
     <t>Lock nut M6</t>
   </si>
   <si>
@@ -282,6 +240,126 @@
   </si>
   <si>
     <t>Bolt</t>
+  </si>
+  <si>
+    <t>tube contains 10 magnets - 2 per feeder needed</t>
+  </si>
+  <si>
+    <t>Vero PureWhite (RGD837) </t>
+  </si>
+  <si>
+    <t>521-945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bag of 100 </t>
+  </si>
+  <si>
+    <t>Washer M6</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Washer</t>
+  </si>
+  <si>
+    <t>797-6257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor </t>
+  </si>
+  <si>
+    <t>Beam break</t>
+  </si>
+  <si>
+    <t>Acrylic</t>
+  </si>
+  <si>
+    <t>Acrylic white matt 3mm</t>
+  </si>
+  <si>
+    <t>Direct Plastics</t>
+  </si>
+  <si>
+    <t>Unidirectional bearing</t>
+  </si>
+  <si>
+    <t>Bearing</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Feeder electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic encoder </t>
+  </si>
+  <si>
+    <t>2619S024SR 361:1</t>
+  </si>
+  <si>
+    <t>Faulhaber</t>
+  </si>
+  <si>
+    <t>Harp</t>
+  </si>
+  <si>
+    <t>OEPS-1113</t>
+  </si>
+  <si>
+    <t>Open ephys</t>
+  </si>
+  <si>
+    <t>Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Raspberry Pi pico V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicone tube </t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>Github for components</t>
+  </si>
+  <si>
+    <t>Custom feeder electronics</t>
+  </si>
+  <si>
+    <t>Custom beam break</t>
+  </si>
+  <si>
+    <t>Thames stock holders</t>
+  </si>
+  <si>
+    <t>AW6082-T6</t>
+  </si>
+  <si>
+    <t>Metal tile</t>
+  </si>
+  <si>
+    <t>3D printer</t>
+  </si>
+  <si>
+    <t>3D printed material</t>
+  </si>
+  <si>
+    <t>273-2493</t>
+  </si>
+  <si>
+    <t>10m roll</t>
+  </si>
+  <si>
+    <t>SKF 6082RSL</t>
+  </si>
+  <si>
+    <t>Simply bearings</t>
+  </si>
+  <si>
+    <t>Stieber CSK8</t>
   </si>
 </sst>
 </file>
@@ -291,7 +369,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,10 +422,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -377,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -396,15 +481,60 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -657,6 +787,166 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -671,8 +961,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{284E5EE1-8247-4A9E-8A15-28ED14FEFFE3}" name="Table22" displayName="Table22" ref="A3:K19" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:K19" xr:uid="{13B3694B-3A36-45DF-BF5F-9F26AAA63BF0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{284E5EE1-8247-4A9E-8A15-28ED14FEFFE3}" name="Table22" displayName="Table22" ref="A3:K32" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A3:K32" xr:uid="{13B3694B-3A36-45DF-BF5F-9F26AAA63BF0}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{82B6A6DF-73AB-4DE4-A7A2-702EF34695E6}" name="Item name "/>
     <tableColumn id="2" xr3:uid="{307439FD-7504-4F39-BED2-D32B3A588652}" name="Item category"/>
@@ -681,8 +971,8 @@
     <tableColumn id="5" xr3:uid="{CCE48749-080D-4FE9-9042-F0DF3B53CAAF}" name="Supplier"/>
     <tableColumn id="12" xr3:uid="{56EE871C-3FDD-41CB-87DC-29F4BD95605A}" name="Quantity per feeder"/>
     <tableColumn id="6" xr3:uid="{F249F6EC-4D15-4366-BF6B-41FEDC495D95}" name="Quantity "/>
-    <tableColumn id="7" xr3:uid="{987B55A7-D983-4B72-8D92-6E78CE707987}" name="Unit price" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{C6227936-0B88-44FB-A21D-C5F5F3B8E818}" name="Total price" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{987B55A7-D983-4B72-8D92-6E78CE707987}" name="Unit price" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{C6227936-0B88-44FB-A21D-C5F5F3B8E818}" name="Total price" dataDxfId="4">
       <calculatedColumnFormula>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{4E03CD8E-8CE4-4DC9-80A4-BE598853D60E}" name="Link"/>
@@ -988,18 +1278,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5038C04-F61F-442E-B660-EA7B254635E8}">
-  <dimension ref="A1:K19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5038C04-F61F-442E-B660-EA7B254635E8}">
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.21875" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" customWidth="1"/>
     <col min="4" max="4" width="27.88671875" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
@@ -1011,17 +1301,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2">
-        <f>SUM(I4:I19)</f>
-        <v>149.71999999999994</v>
+        <f>SUM(I4:I28)</f>
+        <v>322.27999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1041,7 +1331,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>7</v>
@@ -1064,7 +1354,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
@@ -1092,21 +1382,21 @@
         <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -1125,24 +1415,24 @@
         <v>17.47</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -1161,27 +1451,27 @@
         <v>6.07</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>24</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -1197,27 +1487,27 @@
         <v>2.0099999999999998</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
       </c>
       <c r="F8">
         <v>6</v>
@@ -1233,63 +1523,63 @@
         <v>16.97</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <v>14.84</v>
+        <v>7.83</v>
       </c>
       <c r="I9" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>14.84</v>
+        <v>7.83</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <v>6</v>
@@ -1298,53 +1588,53 @@
         <v>1</v>
       </c>
       <c r="H10" s="2">
-        <v>7.83</v>
+        <v>2.19</v>
       </c>
       <c r="I10" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>7.83</v>
+        <v>2.19</v>
       </c>
       <c r="J10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" t="s">
         <v>35</v>
-      </c>
-      <c r="K10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" s="2">
-        <v>2.19</v>
+        <v>8.44</v>
       </c>
       <c r="I11" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>2.19</v>
+        <v>8.44</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1352,16 +1642,16 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F12">
         <v>2</v>
@@ -1370,70 +1660,70 @@
         <v>1</v>
       </c>
       <c r="H12" s="2">
-        <v>8.44</v>
+        <v>5.12</v>
       </c>
       <c r="I12" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>8.44</v>
+        <v>5.12</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>41</v>
       </c>
       <c r="K12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" s="2">
-        <v>5.12</v>
+        <v>2.74</v>
       </c>
       <c r="I13" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>5.12</v>
+        <v>2.74</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -1442,53 +1732,53 @@
         <v>1</v>
       </c>
       <c r="H14" s="2">
-        <v>2.74</v>
+        <v>27.01</v>
       </c>
       <c r="I14" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>2.74</v>
+        <v>27.01</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" s="2">
-        <v>27.01</v>
+        <v>13.39</v>
       </c>
       <c r="I15" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>27.01</v>
+        <v>13.39</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1496,10 +1786,10 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>53</v>
@@ -1508,59 +1798,59 @@
         <v>13</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" s="2">
-        <v>13.39</v>
+        <v>11.76</v>
       </c>
       <c r="I16" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>13.39</v>
+        <v>11.76</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>53</v>
       </c>
       <c r="K16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" s="2">
-        <v>11.76</v>
+        <v>2.64</v>
       </c>
       <c r="I17" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>11.76</v>
+        <v>2.64</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1568,16 +1858,16 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <v>2</v>
@@ -1586,53 +1876,441 @@
         <v>1</v>
       </c>
       <c r="H18" s="2">
-        <v>2.64</v>
+        <v>3.23</v>
       </c>
       <c r="I18" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>2.64</v>
+        <v>3.23</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>59</v>
       </c>
       <c r="K18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" s="2">
-        <v>3.23</v>
+        <v>15.24</v>
       </c>
       <c r="I19" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>3.23</v>
+        <v>15.24</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="K19" t="s">
-        <v>63</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5.87</v>
+      </c>
+      <c r="I20" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>5.87</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>34.85</v>
+      </c>
+      <c r="I21" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>34.85</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="K21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>67.56</v>
+      </c>
+      <c r="I23" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>67.56</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>4</v>
+      </c>
+      <c r="I24" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>4</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2">
+        <v>39.880000000000003</v>
+      </c>
+      <c r="I27" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>39.880000000000003</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>20</v>
+      </c>
+      <c r="I28" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>20</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>22.23</v>
+      </c>
+      <c r="I29" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>22.23</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>5.78</v>
+      </c>
+      <c r="I30" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>5.78</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="I32" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1640,113 +2318,213 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="A4:B19 D4:D19 G4:J19">
-    <cfRule type="expression" dxfId="24" priority="35">
+  <conditionalFormatting sqref="G28:I30 A21:A27 A4:B20 G4:J27 D4:D27">
+    <cfRule type="expression" dxfId="44" priority="59">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="expression" dxfId="43" priority="45">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="42" priority="44">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12 D28:F28 F29:F30">
+    <cfRule type="expression" dxfId="41" priority="43">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="expression" dxfId="23" priority="21">
+    <cfRule type="expression" dxfId="40" priority="42">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="22" priority="20">
+    <cfRule type="expression" dxfId="39" priority="41">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="21" priority="19">
+    <cfRule type="expression" dxfId="38" priority="40">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="20" priority="18">
+    <cfRule type="expression" dxfId="37" priority="39">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="expression" dxfId="36" priority="38">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="19" priority="17">
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="expression" dxfId="34" priority="36">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="expression" dxfId="18" priority="16">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="17" priority="15">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="16" priority="14">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="15" priority="13">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="14" priority="12">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
-    <cfRule type="expression" dxfId="13" priority="11">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
+    <cfRule type="expression" dxfId="33" priority="35">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14">
+    <cfRule type="expression" dxfId="32" priority="34">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="expression" dxfId="31" priority="33">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="30" priority="32">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16">
+    <cfRule type="expression" dxfId="29" priority="31">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="expression" dxfId="28" priority="30">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="expression" dxfId="27" priority="29">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="26" priority="28">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="25" priority="27">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="expression" dxfId="24" priority="26">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="expression" dxfId="23" priority="25">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:B24">
+    <cfRule type="expression" dxfId="22" priority="24">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="expression" dxfId="21" priority="23">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="expression" dxfId="20" priority="22">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:B28 A30">
+    <cfRule type="expression" dxfId="19" priority="19">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28">
+    <cfRule type="expression" dxfId="18" priority="18">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="expression" dxfId="17" priority="17">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="expression" dxfId="16" priority="16">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="expression" dxfId="15" priority="15">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="expression" dxfId="14" priority="14">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="expression" dxfId="13" priority="13">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
     <cfRule type="expression" dxfId="12" priority="10">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
+  <conditionalFormatting sqref="E27">
     <cfRule type="expression" dxfId="11" priority="9">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
+  <conditionalFormatting sqref="A31:A32">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J17">
+  <conditionalFormatting sqref="B31:B32">
     <cfRule type="expression" dxfId="9" priority="7">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
+  <conditionalFormatting sqref="J31:J32">
     <cfRule type="expression" dxfId="8" priority="6">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
+  <conditionalFormatting sqref="K31">
     <cfRule type="expression" dxfId="7" priority="5">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="6" priority="4">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="5" priority="3">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="J30">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1760,35 +2538,54 @@
     <hyperlink ref="J7" r:id="rId4" xr:uid="{9BCB35A8-FDAC-471E-A800-3B83D369BC24}"/>
     <hyperlink ref="D7" location="Feeder!A1" tooltip="Machine Screw Pozi Countersunk M2 x 5mm in A4 Stainless" display="Pozi CSK M2 5" xr:uid="{31A8AB85-C1F4-441C-8871-A6397DD720DD}"/>
     <hyperlink ref="J8" r:id="rId5" xr:uid="{CEDFC72F-5CDF-41E7-9A27-2CDC3097A480}"/>
-    <hyperlink ref="J9" r:id="rId6" xr:uid="{A352D815-B3F9-4D2E-A906-DCE02A329371}"/>
-    <hyperlink ref="D9" location="Feeder!A1" tooltip="RS PRO, Plain Lock Nut, DIN 985, M6" display="Lock nut M6" xr:uid="{9EF552C7-9081-4273-AEBD-558216796FC4}"/>
     <hyperlink ref="D8" location="Feeder!A1" tooltip="M24 x 100mm Socket Countersunk Screws (ISO 10642) - Marine Stainless Steel (A4)" display="Hex CSK M2 10" xr:uid="{E1F05321-DB9C-4C2A-8EDE-A71D7EE455D2}"/>
-    <hyperlink ref="D10" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, ISO 10642, M3 x 6mm" display="Hex CSK M3 6" xr:uid="{04E9FB42-9C16-4242-9B02-FE7F57A55AB0}"/>
-    <hyperlink ref="J10" r:id="rId7" xr:uid="{D1D9A149-AD9B-489A-8A0C-76BE16FF2A29}"/>
-    <hyperlink ref="J11" r:id="rId8" xr:uid="{904A5B58-8976-4E6A-ADE6-A3E943915067}"/>
-    <hyperlink ref="D11" location="Feeder!A1" tooltip="Machine Screw Pozi Countersunk M2.5 x 4mm in A4 Stainless" display="Pozi CSK M2.5 4" xr:uid="{C169F59C-012C-41F4-BEE4-B5ABE22C7E37}"/>
-    <hyperlink ref="D12" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, DIN 7991, M4 x 10mm" display="Hex CSK M4 10" xr:uid="{442A74F8-DE1B-4E35-AB38-39DEA0F49BC9}"/>
-    <hyperlink ref="J12" r:id="rId9" xr:uid="{53923D64-26EF-4CAB-9807-0DA688DA3B4D}"/>
-    <hyperlink ref="J13" r:id="rId10" xr:uid="{170FCE99-2284-47DA-8219-5E4ACAA13129}"/>
-    <hyperlink ref="D13" location="Feeder!A1" tooltip="Socket Head Cap (Allen) Screw M2 x 6mm in A4 Stainless" display="CAP M2 6" xr:uid="{9F2B7C7E-DE11-43E8-A1C6-1882B8DDA5D2}"/>
-    <hyperlink ref="D14" location="Feeder!A1" tooltip="Machine Screw Pozi Countersunk M3 x 30mm in A4 Stainless" display="Pozi CSK M3 30" xr:uid="{CC130658-9801-4421-A26D-D91B75908D00}"/>
-    <hyperlink ref="J14" r:id="rId11" xr:uid="{BC6FF81F-E8D6-48E9-9AFF-DE09777E3468}"/>
-    <hyperlink ref="D15" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Cap Screw, DIN 912, M4 x 20mm" display="CAP M4 20" xr:uid="{882723A4-4931-4BCE-8C2B-2BEA09ED0EA4}"/>
-    <hyperlink ref="J15" r:id="rId12" xr:uid="{EF3E7EF4-138A-48F5-BB00-26DBCF372F60}"/>
-    <hyperlink ref="J16" r:id="rId13" xr:uid="{D5953C58-0DA8-4412-887A-C9439036F6F5}"/>
-    <hyperlink ref="D16" location="Feeder!A1" tooltip="Plain Stainless Steel Hex Socket Set M3 x 10mm Grub Screw" display="Grub M3 10" xr:uid="{9812ABD8-E04A-452B-AECC-E289407C759E}"/>
-    <hyperlink ref="D17" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, ISO 10642, M4 x 12mm" display="Hex CSK M4 12" xr:uid="{92860097-5D33-4B9B-B1D1-9E4B8FA5A76D}"/>
-    <hyperlink ref="J17" r:id="rId14" xr:uid="{868AA9FC-D1C2-4B25-B010-97DAD432A7C4}"/>
-    <hyperlink ref="D18" location="Feeder!A1" tooltip="Socket Head Cap (Allen) Screw M2 x 4mm in A4 Stainless" display="CAP M2 4" xr:uid="{C88E7DC1-5050-4A69-85D2-02FA00C2E380}"/>
-    <hyperlink ref="J18" r:id="rId15" xr:uid="{455AAFF1-16F9-4365-A7A5-54D9353E72A4}"/>
-    <hyperlink ref="D19" location="Feeder!A1" tooltip="Parallel Pin (Dowel Pin) 3 x 12mm (m6 tol) in A1 Stainless Steel (DIN 7)" display="Parallel PIN M3 12" xr:uid="{EE809188-4C32-4C48-B239-971E13A393CC}"/>
-    <hyperlink ref="J19" r:id="rId16" xr:uid="{37643177-BD72-4E03-B224-9F72C19EDBD9}"/>
+    <hyperlink ref="D9" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, ISO 10642, M3 x 6mm" display="Hex CSK M3 6" xr:uid="{04E9FB42-9C16-4242-9B02-FE7F57A55AB0}"/>
+    <hyperlink ref="J9" r:id="rId6" xr:uid="{D1D9A149-AD9B-489A-8A0C-76BE16FF2A29}"/>
+    <hyperlink ref="J10" r:id="rId7" xr:uid="{904A5B58-8976-4E6A-ADE6-A3E943915067}"/>
+    <hyperlink ref="D10" location="Feeder!A1" tooltip="Machine Screw Pozi Countersunk M2.5 x 4mm in A4 Stainless" display="Pozi CSK M2.5 4" xr:uid="{C169F59C-012C-41F4-BEE4-B5ABE22C7E37}"/>
+    <hyperlink ref="D11" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, DIN 7991, M4 x 10mm" display="Hex CSK M4 10" xr:uid="{442A74F8-DE1B-4E35-AB38-39DEA0F49BC9}"/>
+    <hyperlink ref="J11" r:id="rId8" xr:uid="{53923D64-26EF-4CAB-9807-0DA688DA3B4D}"/>
+    <hyperlink ref="J12" r:id="rId9" xr:uid="{170FCE99-2284-47DA-8219-5E4ACAA13129}"/>
+    <hyperlink ref="D12" location="Feeder!A1" tooltip="Socket Head Cap (Allen) Screw M2 x 6mm in A4 Stainless" display="CAP M2 6" xr:uid="{9F2B7C7E-DE11-43E8-A1C6-1882B8DDA5D2}"/>
+    <hyperlink ref="D13" location="Feeder!A1" tooltip="Machine Screw Pozi Countersunk M3 x 30mm in A4 Stainless" display="Pozi CSK M3 30" xr:uid="{CC130658-9801-4421-A26D-D91B75908D00}"/>
+    <hyperlink ref="J13" r:id="rId10" xr:uid="{BC6FF81F-E8D6-48E9-9AFF-DE09777E3468}"/>
+    <hyperlink ref="D14" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Cap Screw, DIN 912, M4 x 20mm" display="CAP M4 20" xr:uid="{882723A4-4931-4BCE-8C2B-2BEA09ED0EA4}"/>
+    <hyperlink ref="J14" r:id="rId11" xr:uid="{EF3E7EF4-138A-48F5-BB00-26DBCF372F60}"/>
+    <hyperlink ref="J15" r:id="rId12" xr:uid="{D5953C58-0DA8-4412-887A-C9439036F6F5}"/>
+    <hyperlink ref="D15" location="Feeder!A1" tooltip="Plain Stainless Steel Hex Socket Set M3 x 10mm Grub Screw" display="Grub M3 10" xr:uid="{9812ABD8-E04A-452B-AECC-E289407C759E}"/>
+    <hyperlink ref="D16" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, ISO 10642, M4 x 12mm" display="Hex CSK M4 12" xr:uid="{92860097-5D33-4B9B-B1D1-9E4B8FA5A76D}"/>
+    <hyperlink ref="J16" r:id="rId13" xr:uid="{868AA9FC-D1C2-4B25-B010-97DAD432A7C4}"/>
+    <hyperlink ref="D17" location="Feeder!A1" tooltip="Socket Head Cap (Allen) Screw M2 x 4mm in A4 Stainless" display="CAP M2 4" xr:uid="{C88E7DC1-5050-4A69-85D2-02FA00C2E380}"/>
+    <hyperlink ref="J17" r:id="rId14" xr:uid="{455AAFF1-16F9-4365-A7A5-54D9353E72A4}"/>
+    <hyperlink ref="D18" location="Feeder!A1" tooltip="Parallel Pin (Dowel Pin) 3 x 12mm (m6 tol) in A1 Stainless Steel (DIN 7)" display="Parallel PIN M3 12" xr:uid="{EE809188-4C32-4C48-B239-971E13A393CC}"/>
+    <hyperlink ref="J18" r:id="rId15" xr:uid="{37643177-BD72-4E03-B224-9F72C19EDBD9}"/>
+    <hyperlink ref="J19" r:id="rId16" xr:uid="{AB0E6DD3-797B-47D3-AAC8-5963B56C13F9}"/>
+    <hyperlink ref="D19" location="Feeder!A1" tooltip="RS PRO Stainless Steel Lock Nut, DIN 985, M6" display="Lock nut M6" xr:uid="{F6DBA852-4B35-40EE-A353-E93A517E65D9}"/>
+    <hyperlink ref="J20" r:id="rId17" xr:uid="{88C0F702-9208-44E0-B8C0-381AE19B3524}"/>
+    <hyperlink ref="D20" location="Feeder!A1" tooltip="A2 304 Stainless Steel Plain Washers, M6, DIN 9021" display="Washer M6" xr:uid="{4142598F-16D4-4341-9C72-462BC4709B95}"/>
+    <hyperlink ref="D28" location="Arena!A1" tooltip="Acrylic White MAtt 3mm Sheet 730mm x 430mm" display="Acrylic white matt 3mm" xr:uid="{02AE9EC4-21BA-439A-A2ED-4BC5A8239E57}"/>
+    <hyperlink ref="J28" r:id="rId18" xr:uid="{71DCD5D2-12DF-4DD5-9863-C375F4C48124}"/>
+    <hyperlink ref="D22" location="Feeder!A1" tooltip="DC-Gearmotors" display="Motor " xr:uid="{0F94B3D2-D79C-450D-AC36-5CD407DF842F}"/>
+    <hyperlink ref="J22" r:id="rId19" location="431" xr:uid="{DCB6954A-27F2-42B1-B6EF-0DA9D562612C}"/>
+    <hyperlink ref="J23" r:id="rId20" xr:uid="{8DBE2A15-54B5-474E-A139-AC6E9C356E5A}"/>
+    <hyperlink ref="J24" r:id="rId21" location="pico-1-technical-specification" xr:uid="{11F0F085-214C-4E04-99A2-5E65F3FDE936}"/>
+    <hyperlink ref="J25" r:id="rId22" xr:uid="{44481561-9533-48EA-9783-F300131B88FE}"/>
+    <hyperlink ref="J26" r:id="rId23" xr:uid="{BB600C18-F5D0-48E5-B1A7-311C75B86686}"/>
+    <hyperlink ref="J27" r:id="rId24" xr:uid="{641A37AD-1654-477A-944A-A2D521139F0E}"/>
+    <hyperlink ref="K32" r:id="rId25" xr:uid="{3AA79703-8ACA-409A-88BC-DAF21F8B3831}"/>
+    <hyperlink ref="J32" r:id="rId26" xr:uid="{55A1D0CD-133D-447B-9C04-2BD5D0FE2887}"/>
+    <hyperlink ref="J31" r:id="rId27" xr:uid="{43DEC2EA-0BE9-4065-90BA-F5A11A691C53}"/>
+    <hyperlink ref="J21" r:id="rId28" xr:uid="{776E0E1E-A99D-46E5-BEDF-A29C724F4651}"/>
+    <hyperlink ref="D21" location="'AEON Feeder'!A1" tooltip="RS PRO Silicone, Flexible Tubing, 1.6mm ID, 3.2mm OD, Translucent, 10m" display="Silicone tube " xr:uid="{3BC53949-ACCC-41BF-86E8-3267F618124D}"/>
+    <hyperlink ref="J30" r:id="rId29" xr:uid="{C4976168-08DB-4607-8D85-96A8E8358D2C}"/>
+    <hyperlink ref="D29" location="'AEON Feeder'!A1" tooltip="CSK8 8mm Sprag Clutch One Way Bearing Without Keyways 8x22x9mm" display="Unidirectional bearing" xr:uid="{EA514DC5-15FB-4BBB-8CD3-5ACD76C7AAD7}"/>
+    <hyperlink ref="D30" location="'AEON Feeder'!A1" tooltip="SKF 6082RSL Deep Groove Ball Bearing with Two Low Friction Rubber Seals 8x22x7mm" display="Bearing" xr:uid="{F3453BA1-8D67-4077-A257-4BE980B927EF}"/>
+    <hyperlink ref="J29" r:id="rId30" xr:uid="{15460AE1-DF6D-449B-B969-1F99FC2DCA6D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
-  <legacyDrawing r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
   <tableParts count="1">
-    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId32"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update hardware modules documentation (#114)
* Add commutation-translation system docs

* Update foraging patch hardware doc

* Update habitat hardware doc

* Update nest hardware doc

* Use 2x2 grid on hardware overview page
</commit_message>
<xml_diff>
--- a/src/downloads/Foraging-Patch-BOM.xlsx
+++ b/src/downloads/Foraging-Patch-BOM.xlsx
@@ -5,15 +5,15 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/412ba1c02c359b1c/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcalc\UCL Dropbox\Lorenza Calcaterra\Project_aeon\Assembly instructions\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{5049CA79-1E51-4C0B-9C8F-9497E3DA38C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F90A9FA6-6850-4C60-80D6-961F114AC47E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF494D9-4B22-4719-887A-C80003F011C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38A5E6C9-8D94-40D2-9BFA-B29F5FB44878}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feeder" sheetId="3" r:id="rId1"/>
+    <sheet name="AEON Feeder" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,44 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Lorenza Calcaterra</author>
-  </authors>
-  <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{EF889EDA-5804-4EB4-9EBB-1F5D632C2E24}">
-      <text/>
-    </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{87F21182-8E0A-403E-B42C-2342DC3F76EA}">
-      <text/>
-    </comment>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{14503D7F-3F9C-4269-9DA8-1D1A15D4BA7C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{6F2DC094-F40F-4E2C-B647-E2E15F32BE0E}">
-      <text/>
-    </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{5CCB3F11-C5AF-4186-97A6-A0003DD56BA7}">
-      <text/>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="108">
   <si>
     <t xml:space="preserve">Inventory list </t>
   </si>
@@ -119,9 +83,6 @@
     <t>Neodymium magnet</t>
   </si>
   <si>
-    <t>tube conains 10 magnets - 2 per feeder needed</t>
-  </si>
-  <si>
     <t>Shoulder bolt</t>
   </si>
   <si>
@@ -167,9 +128,6 @@
     <t>bag of 50 - feeder to hex tile</t>
   </si>
   <si>
-    <t>521-957</t>
-  </si>
-  <si>
     <t>Lock nut M6</t>
   </si>
   <si>
@@ -282,6 +240,126 @@
   </si>
   <si>
     <t>Bolt</t>
+  </si>
+  <si>
+    <t>tube contains 10 magnets - 2 per feeder needed</t>
+  </si>
+  <si>
+    <t>Vero PureWhite (RGD837) </t>
+  </si>
+  <si>
+    <t>521-945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bag of 100 </t>
+  </si>
+  <si>
+    <t>Washer M6</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Washer</t>
+  </si>
+  <si>
+    <t>797-6257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor </t>
+  </si>
+  <si>
+    <t>Beam break</t>
+  </si>
+  <si>
+    <t>Acrylic</t>
+  </si>
+  <si>
+    <t>Acrylic white matt 3mm</t>
+  </si>
+  <si>
+    <t>Direct Plastics</t>
+  </si>
+  <si>
+    <t>Unidirectional bearing</t>
+  </si>
+  <si>
+    <t>Bearing</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Feeder electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic encoder </t>
+  </si>
+  <si>
+    <t>2619S024SR 361:1</t>
+  </si>
+  <si>
+    <t>Faulhaber</t>
+  </si>
+  <si>
+    <t>Harp</t>
+  </si>
+  <si>
+    <t>OEPS-1113</t>
+  </si>
+  <si>
+    <t>Open ephys</t>
+  </si>
+  <si>
+    <t>Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Raspberry Pi pico V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicone tube </t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>Github for components</t>
+  </si>
+  <si>
+    <t>Custom feeder electronics</t>
+  </si>
+  <si>
+    <t>Custom beam break</t>
+  </si>
+  <si>
+    <t>Thames stock holders</t>
+  </si>
+  <si>
+    <t>AW6082-T6</t>
+  </si>
+  <si>
+    <t>Metal tile</t>
+  </si>
+  <si>
+    <t>3D printer</t>
+  </si>
+  <si>
+    <t>3D printed material</t>
+  </si>
+  <si>
+    <t>273-2493</t>
+  </si>
+  <si>
+    <t>10m roll</t>
+  </si>
+  <si>
+    <t>SKF 6082RSL</t>
+  </si>
+  <si>
+    <t>Simply bearings</t>
+  </si>
+  <si>
+    <t>Stieber CSK8</t>
   </si>
 </sst>
 </file>
@@ -291,7 +369,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,10 +422,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -377,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -396,15 +481,60 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -657,6 +787,166 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -671,8 +961,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{284E5EE1-8247-4A9E-8A15-28ED14FEFFE3}" name="Table22" displayName="Table22" ref="A3:K19" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:K19" xr:uid="{13B3694B-3A36-45DF-BF5F-9F26AAA63BF0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{284E5EE1-8247-4A9E-8A15-28ED14FEFFE3}" name="Table22" displayName="Table22" ref="A3:K32" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A3:K32" xr:uid="{13B3694B-3A36-45DF-BF5F-9F26AAA63BF0}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{82B6A6DF-73AB-4DE4-A7A2-702EF34695E6}" name="Item name "/>
     <tableColumn id="2" xr3:uid="{307439FD-7504-4F39-BED2-D32B3A588652}" name="Item category"/>
@@ -681,8 +971,8 @@
     <tableColumn id="5" xr3:uid="{CCE48749-080D-4FE9-9042-F0DF3B53CAAF}" name="Supplier"/>
     <tableColumn id="12" xr3:uid="{56EE871C-3FDD-41CB-87DC-29F4BD95605A}" name="Quantity per feeder"/>
     <tableColumn id="6" xr3:uid="{F249F6EC-4D15-4366-BF6B-41FEDC495D95}" name="Quantity "/>
-    <tableColumn id="7" xr3:uid="{987B55A7-D983-4B72-8D92-6E78CE707987}" name="Unit price" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{C6227936-0B88-44FB-A21D-C5F5F3B8E818}" name="Total price" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{987B55A7-D983-4B72-8D92-6E78CE707987}" name="Unit price" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{C6227936-0B88-44FB-A21D-C5F5F3B8E818}" name="Total price" dataDxfId="4">
       <calculatedColumnFormula>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{4E03CD8E-8CE4-4DC9-80A4-BE598853D60E}" name="Link"/>
@@ -988,18 +1278,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5038C04-F61F-442E-B660-EA7B254635E8}">
-  <dimension ref="A1:K19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5038C04-F61F-442E-B660-EA7B254635E8}">
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.21875" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" customWidth="1"/>
     <col min="4" max="4" width="27.88671875" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
@@ -1011,17 +1301,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2">
-        <f>SUM(I4:I19)</f>
-        <v>149.71999999999994</v>
+        <f>SUM(I4:I28)</f>
+        <v>322.27999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1041,7 +1331,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>7</v>
@@ -1064,7 +1354,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
@@ -1092,21 +1382,21 @@
         <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -1125,24 +1415,24 @@
         <v>17.47</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -1161,27 +1451,27 @@
         <v>6.07</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>24</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -1197,27 +1487,27 @@
         <v>2.0099999999999998</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
       </c>
       <c r="F8">
         <v>6</v>
@@ -1233,63 +1523,63 @@
         <v>16.97</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <v>14.84</v>
+        <v>7.83</v>
       </c>
       <c r="I9" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>14.84</v>
+        <v>7.83</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <v>6</v>
@@ -1298,53 +1588,53 @@
         <v>1</v>
       </c>
       <c r="H10" s="2">
-        <v>7.83</v>
+        <v>2.19</v>
       </c>
       <c r="I10" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>7.83</v>
+        <v>2.19</v>
       </c>
       <c r="J10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" t="s">
         <v>35</v>
-      </c>
-      <c r="K10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" s="2">
-        <v>2.19</v>
+        <v>8.44</v>
       </c>
       <c r="I11" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>2.19</v>
+        <v>8.44</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1352,16 +1642,16 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F12">
         <v>2</v>
@@ -1370,70 +1660,70 @@
         <v>1</v>
       </c>
       <c r="H12" s="2">
-        <v>8.44</v>
+        <v>5.12</v>
       </c>
       <c r="I12" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>8.44</v>
+        <v>5.12</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>41</v>
       </c>
       <c r="K12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" s="2">
-        <v>5.12</v>
+        <v>2.74</v>
       </c>
       <c r="I13" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>5.12</v>
+        <v>2.74</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -1442,53 +1732,53 @@
         <v>1</v>
       </c>
       <c r="H14" s="2">
-        <v>2.74</v>
+        <v>27.01</v>
       </c>
       <c r="I14" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>2.74</v>
+        <v>27.01</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" s="2">
-        <v>27.01</v>
+        <v>13.39</v>
       </c>
       <c r="I15" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>27.01</v>
+        <v>13.39</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1496,10 +1786,10 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>53</v>
@@ -1508,59 +1798,59 @@
         <v>13</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" s="2">
-        <v>13.39</v>
+        <v>11.76</v>
       </c>
       <c r="I16" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>13.39</v>
+        <v>11.76</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>53</v>
       </c>
       <c r="K16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" s="2">
-        <v>11.76</v>
+        <v>2.64</v>
       </c>
       <c r="I17" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>11.76</v>
+        <v>2.64</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1568,16 +1858,16 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <v>2</v>
@@ -1586,53 +1876,441 @@
         <v>1</v>
       </c>
       <c r="H18" s="2">
-        <v>2.64</v>
+        <v>3.23</v>
       </c>
       <c r="I18" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>2.64</v>
+        <v>3.23</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>59</v>
       </c>
       <c r="K18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" s="2">
-        <v>3.23</v>
+        <v>15.24</v>
       </c>
       <c r="I19" s="2">
         <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
-        <v>3.23</v>
+        <v>15.24</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="K19" t="s">
-        <v>63</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5.87</v>
+      </c>
+      <c r="I20" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>5.87</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>34.85</v>
+      </c>
+      <c r="I21" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>34.85</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="K21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>67.56</v>
+      </c>
+      <c r="I23" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>67.56</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>4</v>
+      </c>
+      <c r="I24" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>4</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2">
+        <v>39.880000000000003</v>
+      </c>
+      <c r="I27" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>39.880000000000003</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>20</v>
+      </c>
+      <c r="I28" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>20</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>22.23</v>
+      </c>
+      <c r="I29" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>22.23</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>5.78</v>
+      </c>
+      <c r="I30" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>5.78</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="I32" s="2">
+        <f>Table22[[#This Row],[Quantity ]]*Table22[[#This Row],[Unit price]]</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1640,113 +2318,213 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="A4:B19 D4:D19 G4:J19">
-    <cfRule type="expression" dxfId="24" priority="35">
+  <conditionalFormatting sqref="G28:I30 A21:A27 A4:B20 G4:J27 D4:D27">
+    <cfRule type="expression" dxfId="44" priority="59">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="expression" dxfId="43" priority="45">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="42" priority="44">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12 D28:F28 F29:F30">
+    <cfRule type="expression" dxfId="41" priority="43">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="expression" dxfId="23" priority="21">
+    <cfRule type="expression" dxfId="40" priority="42">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="22" priority="20">
+    <cfRule type="expression" dxfId="39" priority="41">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="21" priority="19">
+    <cfRule type="expression" dxfId="38" priority="40">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="20" priority="18">
+    <cfRule type="expression" dxfId="37" priority="39">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="expression" dxfId="36" priority="38">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="19" priority="17">
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="expression" dxfId="34" priority="36">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="expression" dxfId="18" priority="16">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="17" priority="15">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="16" priority="14">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="15" priority="13">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="14" priority="12">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
-    <cfRule type="expression" dxfId="13" priority="11">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
+    <cfRule type="expression" dxfId="33" priority="35">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14">
+    <cfRule type="expression" dxfId="32" priority="34">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="expression" dxfId="31" priority="33">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="30" priority="32">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16">
+    <cfRule type="expression" dxfId="29" priority="31">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="expression" dxfId="28" priority="30">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="expression" dxfId="27" priority="29">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="26" priority="28">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="25" priority="27">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="expression" dxfId="24" priority="26">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="expression" dxfId="23" priority="25">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:B24">
+    <cfRule type="expression" dxfId="22" priority="24">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="expression" dxfId="21" priority="23">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="expression" dxfId="20" priority="22">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:B28 A30">
+    <cfRule type="expression" dxfId="19" priority="19">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28">
+    <cfRule type="expression" dxfId="18" priority="18">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="expression" dxfId="17" priority="17">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="expression" dxfId="16" priority="16">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="expression" dxfId="15" priority="15">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="expression" dxfId="14" priority="14">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="expression" dxfId="13" priority="13">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
     <cfRule type="expression" dxfId="12" priority="10">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
+  <conditionalFormatting sqref="E27">
     <cfRule type="expression" dxfId="11" priority="9">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
+  <conditionalFormatting sqref="A31:A32">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J17">
+  <conditionalFormatting sqref="B31:B32">
     <cfRule type="expression" dxfId="9" priority="7">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
+  <conditionalFormatting sqref="J31:J32">
     <cfRule type="expression" dxfId="8" priority="6">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
+  <conditionalFormatting sqref="K31">
     <cfRule type="expression" dxfId="7" priority="5">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="6" priority="4">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="5" priority="3">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>#REF!="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="J30">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>#REF!="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!="No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1760,35 +2538,54 @@
     <hyperlink ref="J7" r:id="rId4" xr:uid="{9BCB35A8-FDAC-471E-A800-3B83D369BC24}"/>
     <hyperlink ref="D7" location="Feeder!A1" tooltip="Machine Screw Pozi Countersunk M2 x 5mm in A4 Stainless" display="Pozi CSK M2 5" xr:uid="{31A8AB85-C1F4-441C-8871-A6397DD720DD}"/>
     <hyperlink ref="J8" r:id="rId5" xr:uid="{CEDFC72F-5CDF-41E7-9A27-2CDC3097A480}"/>
-    <hyperlink ref="J9" r:id="rId6" xr:uid="{A352D815-B3F9-4D2E-A906-DCE02A329371}"/>
-    <hyperlink ref="D9" location="Feeder!A1" tooltip="RS PRO, Plain Lock Nut, DIN 985, M6" display="Lock nut M6" xr:uid="{9EF552C7-9081-4273-AEBD-558216796FC4}"/>
     <hyperlink ref="D8" location="Feeder!A1" tooltip="M24 x 100mm Socket Countersunk Screws (ISO 10642) - Marine Stainless Steel (A4)" display="Hex CSK M2 10" xr:uid="{E1F05321-DB9C-4C2A-8EDE-A71D7EE455D2}"/>
-    <hyperlink ref="D10" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, ISO 10642, M3 x 6mm" display="Hex CSK M3 6" xr:uid="{04E9FB42-9C16-4242-9B02-FE7F57A55AB0}"/>
-    <hyperlink ref="J10" r:id="rId7" xr:uid="{D1D9A149-AD9B-489A-8A0C-76BE16FF2A29}"/>
-    <hyperlink ref="J11" r:id="rId8" xr:uid="{904A5B58-8976-4E6A-ADE6-A3E943915067}"/>
-    <hyperlink ref="D11" location="Feeder!A1" tooltip="Machine Screw Pozi Countersunk M2.5 x 4mm in A4 Stainless" display="Pozi CSK M2.5 4" xr:uid="{C169F59C-012C-41F4-BEE4-B5ABE22C7E37}"/>
-    <hyperlink ref="D12" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, DIN 7991, M4 x 10mm" display="Hex CSK M4 10" xr:uid="{442A74F8-DE1B-4E35-AB38-39DEA0F49BC9}"/>
-    <hyperlink ref="J12" r:id="rId9" xr:uid="{53923D64-26EF-4CAB-9807-0DA688DA3B4D}"/>
-    <hyperlink ref="J13" r:id="rId10" xr:uid="{170FCE99-2284-47DA-8219-5E4ACAA13129}"/>
-    <hyperlink ref="D13" location="Feeder!A1" tooltip="Socket Head Cap (Allen) Screw M2 x 6mm in A4 Stainless" display="CAP M2 6" xr:uid="{9F2B7C7E-DE11-43E8-A1C6-1882B8DDA5D2}"/>
-    <hyperlink ref="D14" location="Feeder!A1" tooltip="Machine Screw Pozi Countersunk M3 x 30mm in A4 Stainless" display="Pozi CSK M3 30" xr:uid="{CC130658-9801-4421-A26D-D91B75908D00}"/>
-    <hyperlink ref="J14" r:id="rId11" xr:uid="{BC6FF81F-E8D6-48E9-9AFF-DE09777E3468}"/>
-    <hyperlink ref="D15" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Cap Screw, DIN 912, M4 x 20mm" display="CAP M4 20" xr:uid="{882723A4-4931-4BCE-8C2B-2BEA09ED0EA4}"/>
-    <hyperlink ref="J15" r:id="rId12" xr:uid="{EF3E7EF4-138A-48F5-BB00-26DBCF372F60}"/>
-    <hyperlink ref="J16" r:id="rId13" xr:uid="{D5953C58-0DA8-4412-887A-C9439036F6F5}"/>
-    <hyperlink ref="D16" location="Feeder!A1" tooltip="Plain Stainless Steel Hex Socket Set M3 x 10mm Grub Screw" display="Grub M3 10" xr:uid="{9812ABD8-E04A-452B-AECC-E289407C759E}"/>
-    <hyperlink ref="D17" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, ISO 10642, M4 x 12mm" display="Hex CSK M4 12" xr:uid="{92860097-5D33-4B9B-B1D1-9E4B8FA5A76D}"/>
-    <hyperlink ref="J17" r:id="rId14" xr:uid="{868AA9FC-D1C2-4B25-B010-97DAD432A7C4}"/>
-    <hyperlink ref="D18" location="Feeder!A1" tooltip="Socket Head Cap (Allen) Screw M2 x 4mm in A4 Stainless" display="CAP M2 4" xr:uid="{C88E7DC1-5050-4A69-85D2-02FA00C2E380}"/>
-    <hyperlink ref="J18" r:id="rId15" xr:uid="{455AAFF1-16F9-4365-A7A5-54D9353E72A4}"/>
-    <hyperlink ref="D19" location="Feeder!A1" tooltip="Parallel Pin (Dowel Pin) 3 x 12mm (m6 tol) in A1 Stainless Steel (DIN 7)" display="Parallel PIN M3 12" xr:uid="{EE809188-4C32-4C48-B239-971E13A393CC}"/>
-    <hyperlink ref="J19" r:id="rId16" xr:uid="{37643177-BD72-4E03-B224-9F72C19EDBD9}"/>
+    <hyperlink ref="D9" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, ISO 10642, M3 x 6mm" display="Hex CSK M3 6" xr:uid="{04E9FB42-9C16-4242-9B02-FE7F57A55AB0}"/>
+    <hyperlink ref="J9" r:id="rId6" xr:uid="{D1D9A149-AD9B-489A-8A0C-76BE16FF2A29}"/>
+    <hyperlink ref="J10" r:id="rId7" xr:uid="{904A5B58-8976-4E6A-ADE6-A3E943915067}"/>
+    <hyperlink ref="D10" location="Feeder!A1" tooltip="Machine Screw Pozi Countersunk M2.5 x 4mm in A4 Stainless" display="Pozi CSK M2.5 4" xr:uid="{C169F59C-012C-41F4-BEE4-B5ABE22C7E37}"/>
+    <hyperlink ref="D11" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, DIN 7991, M4 x 10mm" display="Hex CSK M4 10" xr:uid="{442A74F8-DE1B-4E35-AB38-39DEA0F49BC9}"/>
+    <hyperlink ref="J11" r:id="rId8" xr:uid="{53923D64-26EF-4CAB-9807-0DA688DA3B4D}"/>
+    <hyperlink ref="J12" r:id="rId9" xr:uid="{170FCE99-2284-47DA-8219-5E4ACAA13129}"/>
+    <hyperlink ref="D12" location="Feeder!A1" tooltip="Socket Head Cap (Allen) Screw M2 x 6mm in A4 Stainless" display="CAP M2 6" xr:uid="{9F2B7C7E-DE11-43E8-A1C6-1882B8DDA5D2}"/>
+    <hyperlink ref="D13" location="Feeder!A1" tooltip="Machine Screw Pozi Countersunk M3 x 30mm in A4 Stainless" display="Pozi CSK M3 30" xr:uid="{CC130658-9801-4421-A26D-D91B75908D00}"/>
+    <hyperlink ref="J13" r:id="rId10" xr:uid="{BC6FF81F-E8D6-48E9-9AFF-DE09777E3468}"/>
+    <hyperlink ref="D14" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Cap Screw, DIN 912, M4 x 20mm" display="CAP M4 20" xr:uid="{882723A4-4931-4BCE-8C2B-2BEA09ED0EA4}"/>
+    <hyperlink ref="J14" r:id="rId11" xr:uid="{EF3E7EF4-138A-48F5-BB00-26DBCF372F60}"/>
+    <hyperlink ref="J15" r:id="rId12" xr:uid="{D5953C58-0DA8-4412-887A-C9439036F6F5}"/>
+    <hyperlink ref="D15" location="Feeder!A1" tooltip="Plain Stainless Steel Hex Socket Set M3 x 10mm Grub Screw" display="Grub M3 10" xr:uid="{9812ABD8-E04A-452B-AECC-E289407C759E}"/>
+    <hyperlink ref="D16" location="Feeder!A1" tooltip="RS PRO Plain Stainless Steel Hex Socket Countersunk Screw, ISO 10642, M4 x 12mm" display="Hex CSK M4 12" xr:uid="{92860097-5D33-4B9B-B1D1-9E4B8FA5A76D}"/>
+    <hyperlink ref="J16" r:id="rId13" xr:uid="{868AA9FC-D1C2-4B25-B010-97DAD432A7C4}"/>
+    <hyperlink ref="D17" location="Feeder!A1" tooltip="Socket Head Cap (Allen) Screw M2 x 4mm in A4 Stainless" display="CAP M2 4" xr:uid="{C88E7DC1-5050-4A69-85D2-02FA00C2E380}"/>
+    <hyperlink ref="J17" r:id="rId14" xr:uid="{455AAFF1-16F9-4365-A7A5-54D9353E72A4}"/>
+    <hyperlink ref="D18" location="Feeder!A1" tooltip="Parallel Pin (Dowel Pin) 3 x 12mm (m6 tol) in A1 Stainless Steel (DIN 7)" display="Parallel PIN M3 12" xr:uid="{EE809188-4C32-4C48-B239-971E13A393CC}"/>
+    <hyperlink ref="J18" r:id="rId15" xr:uid="{37643177-BD72-4E03-B224-9F72C19EDBD9}"/>
+    <hyperlink ref="J19" r:id="rId16" xr:uid="{AB0E6DD3-797B-47D3-AAC8-5963B56C13F9}"/>
+    <hyperlink ref="D19" location="Feeder!A1" tooltip="RS PRO Stainless Steel Lock Nut, DIN 985, M6" display="Lock nut M6" xr:uid="{F6DBA852-4B35-40EE-A353-E93A517E65D9}"/>
+    <hyperlink ref="J20" r:id="rId17" xr:uid="{88C0F702-9208-44E0-B8C0-381AE19B3524}"/>
+    <hyperlink ref="D20" location="Feeder!A1" tooltip="A2 304 Stainless Steel Plain Washers, M6, DIN 9021" display="Washer M6" xr:uid="{4142598F-16D4-4341-9C72-462BC4709B95}"/>
+    <hyperlink ref="D28" location="Arena!A1" tooltip="Acrylic White MAtt 3mm Sheet 730mm x 430mm" display="Acrylic white matt 3mm" xr:uid="{02AE9EC4-21BA-439A-A2ED-4BC5A8239E57}"/>
+    <hyperlink ref="J28" r:id="rId18" xr:uid="{71DCD5D2-12DF-4DD5-9863-C375F4C48124}"/>
+    <hyperlink ref="D22" location="Feeder!A1" tooltip="DC-Gearmotors" display="Motor " xr:uid="{0F94B3D2-D79C-450D-AC36-5CD407DF842F}"/>
+    <hyperlink ref="J22" r:id="rId19" location="431" xr:uid="{DCB6954A-27F2-42B1-B6EF-0DA9D562612C}"/>
+    <hyperlink ref="J23" r:id="rId20" xr:uid="{8DBE2A15-54B5-474E-A139-AC6E9C356E5A}"/>
+    <hyperlink ref="J24" r:id="rId21" location="pico-1-technical-specification" xr:uid="{11F0F085-214C-4E04-99A2-5E65F3FDE936}"/>
+    <hyperlink ref="J25" r:id="rId22" xr:uid="{44481561-9533-48EA-9783-F300131B88FE}"/>
+    <hyperlink ref="J26" r:id="rId23" xr:uid="{BB600C18-F5D0-48E5-B1A7-311C75B86686}"/>
+    <hyperlink ref="J27" r:id="rId24" xr:uid="{641A37AD-1654-477A-944A-A2D521139F0E}"/>
+    <hyperlink ref="K32" r:id="rId25" xr:uid="{3AA79703-8ACA-409A-88BC-DAF21F8B3831}"/>
+    <hyperlink ref="J32" r:id="rId26" xr:uid="{55A1D0CD-133D-447B-9C04-2BD5D0FE2887}"/>
+    <hyperlink ref="J31" r:id="rId27" xr:uid="{43DEC2EA-0BE9-4065-90BA-F5A11A691C53}"/>
+    <hyperlink ref="J21" r:id="rId28" xr:uid="{776E0E1E-A99D-46E5-BEDF-A29C724F4651}"/>
+    <hyperlink ref="D21" location="'AEON Feeder'!A1" tooltip="RS PRO Silicone, Flexible Tubing, 1.6mm ID, 3.2mm OD, Translucent, 10m" display="Silicone tube " xr:uid="{3BC53949-ACCC-41BF-86E8-3267F618124D}"/>
+    <hyperlink ref="J30" r:id="rId29" xr:uid="{C4976168-08DB-4607-8D85-96A8E8358D2C}"/>
+    <hyperlink ref="D29" location="'AEON Feeder'!A1" tooltip="CSK8 8mm Sprag Clutch One Way Bearing Without Keyways 8x22x9mm" display="Unidirectional bearing" xr:uid="{EA514DC5-15FB-4BBB-8CD3-5ACD76C7AAD7}"/>
+    <hyperlink ref="D30" location="'AEON Feeder'!A1" tooltip="SKF 6082RSL Deep Groove Ball Bearing with Two Low Friction Rubber Seals 8x22x7mm" display="Bearing" xr:uid="{F3453BA1-8D67-4077-A257-4BE980B927EF}"/>
+    <hyperlink ref="J29" r:id="rId30" xr:uid="{15460AE1-DF6D-449B-B969-1F99FC2DCA6D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
-  <legacyDrawing r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
   <tableParts count="1">
-    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId32"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>